<commit_message>
UPDATE CustomReport (Sub Report)
</commit_message>
<xml_diff>
--- a/Exported-Reports/CustomReport.xlsx
+++ b/Exported-Reports/CustomReport.xlsx
@@ -34,6 +34,46 @@
       <strike val="false"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="34.0"/>
+      <color rgb="FFFFFF"/>
+      <name val="SansSerif"/>
+      <b val="true"/>
+      <i val="false"/>
+      <u val="none"/>
+      <strike val="false"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FFFFFF"/>
+      <name val="SansSerif"/>
+      <b val="false"/>
+      <i val="false"/>
+      <u val="none"/>
+      <strike val="false"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14.0"/>
+      <color rgb="006699"/>
+      <name val="SansSerif"/>
+      <b val="true"/>
+      <i val="false"/>
+      <u val="none"/>
+      <strike val="false"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14.0"/>
+      <color rgb="000000"/>
+      <name val="SansSerif"/>
+      <b val="false"/>
+      <i val="false"/>
+      <u val="none"/>
+      <strike val="false"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills>
     <fill>
@@ -132,6 +172,46 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="006699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="006699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="006699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="006699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
   </fills>
@@ -192,6 +272,21 @@
       <left>
         <color rgb="000000"/>
       </left>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
       <right style="thin">
         <color rgb="000000"/>
       </right>
@@ -214,6 +309,51 @@
         <color rgb="000000"/>
       </top>
       <bottom style="thin">
+        <color rgb="000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left>
+        <color rgb="FFFFFF"/>
+      </left>
+      <right>
+        <color rgb="FFFFFF"/>
+      </right>
+      <top>
+        <color rgb="FFFFFF"/>
+      </top>
+      <bottom>
+        <color rgb="FFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left>
+        <color rgb="006699"/>
+      </left>
+      <right>
+        <color rgb="006699"/>
+      </right>
+      <top>
+        <color rgb="006699"/>
+      </top>
+      <bottom>
+        <color rgb="006699"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="666666"/>
+      </top>
+      <bottom>
         <color rgb="000000"/>
       </bottom>
       <diagonal/>
@@ -260,11 +400,11 @@
       <alignment wrapText="true"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment wrapText="true" horizontal="center" vertical="center"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment wrapText="true" horizontal="center" vertical="center"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -280,7 +420,7 @@
       <alignment wrapText="true"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="5" xfId="0" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="6" xfId="0" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment wrapText="true" horizontal="center" vertical="center"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -295,6 +435,38 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment wrapText="true"/>
       <protection hidden="false" locked="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment wrapText="true"/>
+      <protection hidden="false" locked="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="7" xfId="0" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment wrapText="true" horizontal="left" vertical="top"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment wrapText="true"/>
+      <protection hidden="false" locked="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="7" xfId="0" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment wrapText="true" horizontal="left" vertical="top"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="8" xfId="0" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment wrapText="true" horizontal="center" vertical="top"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="9" xfId="0" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment wrapText="true"/>
+      <protection hidden="false" locked="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="1" xfId="0" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment wrapText="true" horizontal="center" vertical="top"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="1" xfId="0" applyAlignment="1" applyProtection="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment wrapText="true" horizontal="left" vertical="top"/>
+      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
   <dxfs count="0"/>
@@ -312,14 +484,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1005344801" name="Picture">
+        <xdr:cNvPr id="441867003" name="Picture">
 </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
@@ -344,23 +516,23 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1932303196" name="Picture">
+        <xdr:cNvPr id="1315908533" name="Picture">
 </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="img_0_1_1.png"/>
+        <a:blip r:embed="img_0_2_0.png"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect l="0" t="0" r="0" b="0"/>
@@ -378,25 +550,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1030384622" name="Picture">
+        <xdr:cNvPr id="1063423209" name="Picture">
 </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="img_0_1_2.png"/>
+        <a:blip r:embed="img_0_2_1.png"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect l="0" t="0" r="0" b="0"/>
@@ -427,18 +599,29 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="1" width="3.3333333"/>
-    <col min="2" max="2" customWidth="1" width="13.5"/>
-    <col min="3" max="3" customWidth="1" width="3.1666667"/>
-    <col min="4" max="4" customWidth="1" width="16.666666"/>
-    <col min="5" max="5" customWidth="1" width="5.0"/>
-    <col min="6" max="6" customWidth="1" width="16.666666"/>
-    <col min="7" max="7" customWidth="1" width="4.1666665"/>
-    <col min="8" max="8" customWidth="1" width="4.1666665"/>
-    <col min="9" max="9" customWidth="1" width="12.5"/>
-    <col min="10" max="10" customWidth="1" width="4.1666665"/>
-    <col min="11" max="11" customWidth="1" width="12.333333"/>
-    <col min="12" max="12" customWidth="1" width="0.16666667"/>
-    <col min="13" max="13" customWidth="1" width="3.3333333"/>
+    <col min="2" max="2" customWidth="1" width="3.3333333"/>
+    <col min="3" max="3" customWidth="1" width="10.166667"/>
+    <col min="4" max="4" customWidth="1" width="3.1666667"/>
+    <col min="5" max="5" customWidth="1" width="3.3333333"/>
+    <col min="6" max="6" customWidth="1" width="1.8333334"/>
+    <col min="7" max="7" customWidth="1" width="11.5"/>
+    <col min="8" max="8" customWidth="1" width="5.0"/>
+    <col min="9" max="9" customWidth="1" width="2.0"/>
+    <col min="10" max="10" customWidth="1" width="2.0"/>
+    <col min="11" max="11" customWidth="1" width="12.666667"/>
+    <col min="12" max="12" customWidth="1" width="3.8333333"/>
+    <col min="13" max="13" customWidth="1" width="0.33333334"/>
+    <col min="14" max="14" customWidth="1" width="4.1666665"/>
+    <col min="15" max="15" customWidth="1" width="12.5"/>
+    <col min="16" max="16" customWidth="1" width="1.5"/>
+    <col min="17" max="17" customWidth="1" width="1.0"/>
+    <col min="18" max="18" customWidth="1" width="1.6666666"/>
+    <col min="19" max="19" customWidth="1" width="9.166667"/>
+    <col min="20" max="20" customWidth="1" width="3.1666667"/>
+    <col min="21" max="21" customWidth="1" width="0.16666667"/>
+    <col min="22" max="22" customWidth="1" width="2.5"/>
+    <col min="23" max="23" customWidth="1" width="0.8333333"/>
+    <col min="24" max="24" customWidth="1" width="3.3333333"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" ht="20">
@@ -455,6 +638,17 @@
       <c r="K1" s="1" t="inlineStr"/>
       <c r="L1" s="1" t="inlineStr"/>
       <c r="M1" s="1" t="inlineStr"/>
+      <c r="N1" s="1" t="inlineStr"/>
+      <c r="O1" s="1" t="inlineStr"/>
+      <c r="P1" s="1" t="inlineStr"/>
+      <c r="Q1" s="1" t="inlineStr"/>
+      <c r="R1" s="1" t="inlineStr"/>
+      <c r="S1" s="1" t="inlineStr"/>
+      <c r="T1" s="1" t="inlineStr"/>
+      <c r="U1" s="1" t="inlineStr"/>
+      <c r="V1" s="1" t="inlineStr"/>
+      <c r="W1" s="1" t="inlineStr"/>
+      <c r="X1" s="1" t="inlineStr"/>
     </row>
     <row r="2" customHeight="1" ht="11">
       <c r="A2" s="1" t="inlineStr"/>
@@ -469,33 +663,55 @@
       <c r="J2" s="2" t="inlineStr"/>
       <c r="K2" s="2" t="inlineStr"/>
       <c r="L2" s="2" t="inlineStr"/>
-      <c r="M2" s="1" t="inlineStr"/>
+      <c r="M2" s="2" t="inlineStr"/>
+      <c r="N2" s="2" t="inlineStr"/>
+      <c r="O2" s="2" t="inlineStr"/>
+      <c r="P2" s="2" t="inlineStr"/>
+      <c r="Q2" s="2" t="inlineStr"/>
+      <c r="R2" s="2" t="inlineStr"/>
+      <c r="S2" s="2" t="inlineStr"/>
+      <c r="T2" s="2" t="inlineStr"/>
+      <c r="U2" s="2" t="inlineStr"/>
+      <c r="V2" s="1" t="inlineStr"/>
+      <c r="W2" s="1" t="inlineStr"/>
+      <c r="X2" s="1" t="inlineStr"/>
     </row>
     <row r="3" customHeight="1" ht="30">
       <c r="A3" s="1" t="inlineStr"/>
       <c r="B3" s="2" t="inlineStr"/>
-      <c r="C3" s="3" t="inlineStr"/>
+      <c r="C3" s="2" t="inlineStr"/>
       <c r="D3" s="3" t="inlineStr"/>
       <c r="E3" s="3" t="inlineStr"/>
-      <c r="F3" s="4" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">Student Report</t>
-          </r>
-        </is>
-      </c>
+      <c r="F3" s="3" t="inlineStr"/>
       <c r="G3" s="3" t="inlineStr"/>
       <c r="H3" s="3" t="inlineStr"/>
-      <c r="I3" s="3" t="inlineStr"/>
-      <c r="J3" s="3" t="inlineStr"/>
-      <c r="K3" s="3" t="inlineStr"/>
-      <c r="L3" s="2" t="inlineStr"/>
-      <c r="M3" s="1" t="inlineStr"/>
+      <c r="I3" s="4" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Student Report</t>
+          </r>
+        </is>
+      </c>
+      <c r="J3" s="4" t="inlineStr"/>
+      <c r="K3" s="4" t="inlineStr"/>
+      <c r="L3" s="3" t="inlineStr"/>
+      <c r="M3" s="3" t="inlineStr"/>
+      <c r="N3" s="3" t="inlineStr"/>
+      <c r="O3" s="3" t="inlineStr"/>
+      <c r="P3" s="3" t="inlineStr"/>
+      <c r="Q3" s="3" t="inlineStr"/>
+      <c r="R3" s="3" t="inlineStr"/>
+      <c r="S3" s="3" t="inlineStr"/>
+      <c r="T3" s="3" t="inlineStr"/>
+      <c r="U3" s="2" t="inlineStr"/>
+      <c r="V3" s="1" t="inlineStr"/>
+      <c r="W3" s="1" t="inlineStr"/>
+      <c r="X3" s="1" t="inlineStr"/>
     </row>
     <row r="4" customHeight="1" ht="16">
       <c r="A4" s="1" t="inlineStr"/>
       <c r="B4" s="2" t="inlineStr"/>
-      <c r="C4" s="3" t="inlineStr"/>
+      <c r="C4" s="2" t="inlineStr"/>
       <c r="D4" s="3" t="inlineStr"/>
       <c r="E4" s="3" t="inlineStr"/>
       <c r="F4" s="3" t="inlineStr"/>
@@ -504,8 +720,19 @@
       <c r="I4" s="3" t="inlineStr"/>
       <c r="J4" s="3" t="inlineStr"/>
       <c r="K4" s="3" t="inlineStr"/>
-      <c r="L4" s="2" t="inlineStr"/>
-      <c r="M4" s="1" t="inlineStr"/>
+      <c r="L4" s="3" t="inlineStr"/>
+      <c r="M4" s="3" t="inlineStr"/>
+      <c r="N4" s="3" t="inlineStr"/>
+      <c r="O4" s="3" t="inlineStr"/>
+      <c r="P4" s="3" t="inlineStr"/>
+      <c r="Q4" s="3" t="inlineStr"/>
+      <c r="R4" s="3" t="inlineStr"/>
+      <c r="S4" s="3" t="inlineStr"/>
+      <c r="T4" s="3" t="inlineStr"/>
+      <c r="U4" s="2" t="inlineStr"/>
+      <c r="V4" s="1" t="inlineStr"/>
+      <c r="W4" s="1" t="inlineStr"/>
+      <c r="X4" s="1" t="inlineStr"/>
     </row>
     <row r="5" customHeight="1" ht="30">
       <c r="A5" s="1" t="inlineStr"/>
@@ -516,17 +743,28 @@
       <c r="F5" s="2" t="inlineStr"/>
       <c r="G5" s="2" t="inlineStr"/>
       <c r="H5" s="2" t="inlineStr"/>
-      <c r="I5" s="5" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">John</t>
-          </r>
-        </is>
-      </c>
-      <c r="J5" s="5" t="inlineStr"/>
+      <c r="I5" s="2" t="inlineStr"/>
+      <c r="J5" s="2" t="inlineStr"/>
       <c r="K5" s="2" t="inlineStr"/>
       <c r="L5" s="2" t="inlineStr"/>
-      <c r="M5" s="1" t="inlineStr"/>
+      <c r="M5" s="2" t="inlineStr"/>
+      <c r="N5" s="2" t="inlineStr"/>
+      <c r="O5" s="5" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">John</t>
+          </r>
+        </is>
+      </c>
+      <c r="P5" s="5" t="inlineStr"/>
+      <c r="Q5" s="5" t="inlineStr"/>
+      <c r="R5" s="5" t="inlineStr"/>
+      <c r="S5" s="2" t="inlineStr"/>
+      <c r="T5" s="2" t="inlineStr"/>
+      <c r="U5" s="2" t="inlineStr"/>
+      <c r="V5" s="1" t="inlineStr"/>
+      <c r="W5" s="1" t="inlineStr"/>
+      <c r="X5" s="1" t="inlineStr"/>
     </row>
     <row r="6" customHeight="1" ht="18">
       <c r="A6" s="1" t="inlineStr"/>
@@ -542,6 +780,17 @@
       <c r="K6" s="1" t="inlineStr"/>
       <c r="L6" s="1" t="inlineStr"/>
       <c r="M6" s="1" t="inlineStr"/>
+      <c r="N6" s="1" t="inlineStr"/>
+      <c r="O6" s="1" t="inlineStr"/>
+      <c r="P6" s="1" t="inlineStr"/>
+      <c r="Q6" s="1" t="inlineStr"/>
+      <c r="R6" s="1" t="inlineStr"/>
+      <c r="S6" s="1" t="inlineStr"/>
+      <c r="T6" s="1" t="inlineStr"/>
+      <c r="U6" s="1" t="inlineStr"/>
+      <c r="V6" s="1" t="inlineStr"/>
+      <c r="W6" s="1" t="inlineStr"/>
+      <c r="X6" s="1" t="inlineStr"/>
     </row>
     <row r="7" customHeight="1" ht="1">
       <c r="A7" s="1" t="inlineStr"/>
@@ -556,7 +805,18 @@
       <c r="J7" s="6" t="inlineStr"/>
       <c r="K7" s="6" t="inlineStr"/>
       <c r="L7" s="6" t="inlineStr"/>
-      <c r="M7" s="1" t="inlineStr"/>
+      <c r="M7" s="6" t="inlineStr"/>
+      <c r="N7" s="6" t="inlineStr"/>
+      <c r="O7" s="6" t="inlineStr"/>
+      <c r="P7" s="6" t="inlineStr"/>
+      <c r="Q7" s="6" t="inlineStr"/>
+      <c r="R7" s="6" t="inlineStr"/>
+      <c r="S7" s="6" t="inlineStr"/>
+      <c r="T7" s="6" t="inlineStr"/>
+      <c r="U7" s="6" t="inlineStr"/>
+      <c r="V7" s="1" t="inlineStr"/>
+      <c r="W7" s="1" t="inlineStr"/>
+      <c r="X7" s="1" t="inlineStr"/>
     </row>
     <row r="8" customHeight="1" ht="17">
       <c r="A8" s="1" t="inlineStr"/>
@@ -572,21 +832,43 @@
       <c r="K8" s="1" t="inlineStr"/>
       <c r="L8" s="1" t="inlineStr"/>
       <c r="M8" s="1" t="inlineStr"/>
+      <c r="N8" s="1" t="inlineStr"/>
+      <c r="O8" s="1" t="inlineStr"/>
+      <c r="P8" s="1" t="inlineStr"/>
+      <c r="Q8" s="1" t="inlineStr"/>
+      <c r="R8" s="1" t="inlineStr"/>
+      <c r="S8" s="1" t="inlineStr"/>
+      <c r="T8" s="1" t="inlineStr"/>
+      <c r="U8" s="1" t="inlineStr"/>
+      <c r="V8" s="1" t="inlineStr"/>
+      <c r="W8" s="1" t="inlineStr"/>
+      <c r="X8" s="1" t="inlineStr"/>
     </row>
     <row r="9" customHeight="1" ht="30">
       <c r="A9" s="1" t="inlineStr"/>
       <c r="B9" s="7" t="inlineStr"/>
       <c r="C9" s="8" t="inlineStr"/>
       <c r="D9" s="9" t="inlineStr"/>
-      <c r="E9" s="1" t="inlineStr"/>
-      <c r="F9" s="1" t="inlineStr"/>
-      <c r="G9" s="1" t="inlineStr"/>
+      <c r="E9" s="7" t="inlineStr"/>
+      <c r="F9" s="8" t="inlineStr"/>
+      <c r="G9" s="9" t="inlineStr"/>
       <c r="H9" s="1" t="inlineStr"/>
       <c r="I9" s="1" t="inlineStr"/>
       <c r="J9" s="1" t="inlineStr"/>
       <c r="K9" s="1" t="inlineStr"/>
       <c r="L9" s="1" t="inlineStr"/>
       <c r="M9" s="1" t="inlineStr"/>
+      <c r="N9" s="1" t="inlineStr"/>
+      <c r="O9" s="1" t="inlineStr"/>
+      <c r="P9" s="1" t="inlineStr"/>
+      <c r="Q9" s="1" t="inlineStr"/>
+      <c r="R9" s="1" t="inlineStr"/>
+      <c r="S9" s="1" t="inlineStr"/>
+      <c r="T9" s="1" t="inlineStr"/>
+      <c r="U9" s="1" t="inlineStr"/>
+      <c r="V9" s="1" t="inlineStr"/>
+      <c r="W9" s="1" t="inlineStr"/>
+      <c r="X9" s="1" t="inlineStr"/>
     </row>
     <row r="10" customHeight="1" ht="30">
       <c r="A10" s="1" t="inlineStr"/>
@@ -598,22 +880,33 @@
         </is>
       </c>
       <c r="C10" s="10" t="inlineStr"/>
-      <c r="D10" s="10" t="inlineStr">
+      <c r="D10" s="10" t="inlineStr"/>
+      <c r="E10" s="10" t="inlineStr">
         <is>
           <r>
             <t xml:space="preserve">Marks Obtained</t>
           </r>
         </is>
       </c>
-      <c r="E10" s="1" t="inlineStr"/>
-      <c r="F10" s="1" t="inlineStr"/>
-      <c r="G10" s="1" t="inlineStr"/>
+      <c r="F10" s="10" t="inlineStr"/>
+      <c r="G10" s="10" t="inlineStr"/>
       <c r="H10" s="1" t="inlineStr"/>
       <c r="I10" s="1" t="inlineStr"/>
       <c r="J10" s="1" t="inlineStr"/>
       <c r="K10" s="1" t="inlineStr"/>
       <c r="L10" s="1" t="inlineStr"/>
       <c r="M10" s="1" t="inlineStr"/>
+      <c r="N10" s="1" t="inlineStr"/>
+      <c r="O10" s="1" t="inlineStr"/>
+      <c r="P10" s="1" t="inlineStr"/>
+      <c r="Q10" s="1" t="inlineStr"/>
+      <c r="R10" s="1" t="inlineStr"/>
+      <c r="S10" s="1" t="inlineStr"/>
+      <c r="T10" s="1" t="inlineStr"/>
+      <c r="U10" s="1" t="inlineStr"/>
+      <c r="V10" s="1" t="inlineStr"/>
+      <c r="W10" s="1" t="inlineStr"/>
+      <c r="X10" s="1" t="inlineStr"/>
     </row>
     <row r="11" customHeight="1" ht="30">
       <c r="A11" s="1" t="inlineStr"/>
@@ -625,22 +918,33 @@
         </is>
       </c>
       <c r="C11" s="11" t="inlineStr"/>
-      <c r="D11" s="11" t="inlineStr">
+      <c r="D11" s="11" t="inlineStr"/>
+      <c r="E11" s="11" t="inlineStr">
         <is>
           <r>
             <t xml:space="preserve">60</t>
           </r>
         </is>
       </c>
-      <c r="E11" s="1" t="inlineStr"/>
-      <c r="F11" s="1" t="inlineStr"/>
-      <c r="G11" s="1" t="inlineStr"/>
+      <c r="F11" s="11" t="inlineStr"/>
+      <c r="G11" s="11" t="inlineStr"/>
       <c r="H11" s="1" t="inlineStr"/>
       <c r="I11" s="1" t="inlineStr"/>
       <c r="J11" s="1" t="inlineStr"/>
       <c r="K11" s="1" t="inlineStr"/>
       <c r="L11" s="1" t="inlineStr"/>
       <c r="M11" s="1" t="inlineStr"/>
+      <c r="N11" s="1" t="inlineStr"/>
+      <c r="O11" s="1" t="inlineStr"/>
+      <c r="P11" s="1" t="inlineStr"/>
+      <c r="Q11" s="1" t="inlineStr"/>
+      <c r="R11" s="1" t="inlineStr"/>
+      <c r="S11" s="1" t="inlineStr"/>
+      <c r="T11" s="1" t="inlineStr"/>
+      <c r="U11" s="1" t="inlineStr"/>
+      <c r="V11" s="1" t="inlineStr"/>
+      <c r="W11" s="1" t="inlineStr"/>
+      <c r="X11" s="1" t="inlineStr"/>
     </row>
     <row r="12" customHeight="1" ht="30">
       <c r="A12" s="1" t="inlineStr"/>
@@ -652,22 +956,33 @@
         </is>
       </c>
       <c r="C12" s="11" t="inlineStr"/>
-      <c r="D12" s="11" t="inlineStr">
+      <c r="D12" s="11" t="inlineStr"/>
+      <c r="E12" s="11" t="inlineStr">
         <is>
           <r>
             <t xml:space="preserve">80</t>
           </r>
         </is>
       </c>
-      <c r="E12" s="1" t="inlineStr"/>
-      <c r="F12" s="1" t="inlineStr"/>
-      <c r="G12" s="1" t="inlineStr"/>
+      <c r="F12" s="11" t="inlineStr"/>
+      <c r="G12" s="11" t="inlineStr"/>
       <c r="H12" s="1" t="inlineStr"/>
       <c r="I12" s="1" t="inlineStr"/>
       <c r="J12" s="1" t="inlineStr"/>
       <c r="K12" s="1" t="inlineStr"/>
       <c r="L12" s="1" t="inlineStr"/>
       <c r="M12" s="1" t="inlineStr"/>
+      <c r="N12" s="1" t="inlineStr"/>
+      <c r="O12" s="1" t="inlineStr"/>
+      <c r="P12" s="1" t="inlineStr"/>
+      <c r="Q12" s="1" t="inlineStr"/>
+      <c r="R12" s="1" t="inlineStr"/>
+      <c r="S12" s="1" t="inlineStr"/>
+      <c r="T12" s="1" t="inlineStr"/>
+      <c r="U12" s="1" t="inlineStr"/>
+      <c r="V12" s="1" t="inlineStr"/>
+      <c r="W12" s="1" t="inlineStr"/>
+      <c r="X12" s="1" t="inlineStr"/>
     </row>
     <row r="13" customHeight="1" ht="30">
       <c r="A13" s="1" t="inlineStr"/>
@@ -679,22 +994,33 @@
         </is>
       </c>
       <c r="C13" s="11" t="inlineStr"/>
-      <c r="D13" s="11" t="inlineStr">
+      <c r="D13" s="11" t="inlineStr"/>
+      <c r="E13" s="11" t="inlineStr">
         <is>
           <r>
             <t xml:space="preserve">40</t>
           </r>
         </is>
       </c>
-      <c r="E13" s="1" t="inlineStr"/>
-      <c r="F13" s="1" t="inlineStr"/>
-      <c r="G13" s="1" t="inlineStr"/>
+      <c r="F13" s="11" t="inlineStr"/>
+      <c r="G13" s="11" t="inlineStr"/>
       <c r="H13" s="1" t="inlineStr"/>
       <c r="I13" s="1" t="inlineStr"/>
       <c r="J13" s="1" t="inlineStr"/>
       <c r="K13" s="1" t="inlineStr"/>
       <c r="L13" s="1" t="inlineStr"/>
       <c r="M13" s="1" t="inlineStr"/>
+      <c r="N13" s="1" t="inlineStr"/>
+      <c r="O13" s="1" t="inlineStr"/>
+      <c r="P13" s="1" t="inlineStr"/>
+      <c r="Q13" s="1" t="inlineStr"/>
+      <c r="R13" s="1" t="inlineStr"/>
+      <c r="S13" s="1" t="inlineStr"/>
+      <c r="T13" s="1" t="inlineStr"/>
+      <c r="U13" s="1" t="inlineStr"/>
+      <c r="V13" s="1" t="inlineStr"/>
+      <c r="W13" s="1" t="inlineStr"/>
+      <c r="X13" s="1" t="inlineStr"/>
     </row>
     <row r="14" customHeight="1" ht="30">
       <c r="A14" s="1" t="inlineStr"/>
@@ -706,22 +1032,33 @@
         </is>
       </c>
       <c r="C14" s="11" t="inlineStr"/>
-      <c r="D14" s="11" t="inlineStr">
+      <c r="D14" s="11" t="inlineStr"/>
+      <c r="E14" s="11" t="inlineStr">
         <is>
           <r>
             <t xml:space="preserve">70</t>
           </r>
         </is>
       </c>
-      <c r="E14" s="1" t="inlineStr"/>
-      <c r="F14" s="1" t="inlineStr"/>
-      <c r="G14" s="1" t="inlineStr"/>
+      <c r="F14" s="11" t="inlineStr"/>
+      <c r="G14" s="11" t="inlineStr"/>
       <c r="H14" s="1" t="inlineStr"/>
       <c r="I14" s="1" t="inlineStr"/>
       <c r="J14" s="1" t="inlineStr"/>
       <c r="K14" s="1" t="inlineStr"/>
       <c r="L14" s="1" t="inlineStr"/>
       <c r="M14" s="1" t="inlineStr"/>
+      <c r="N14" s="1" t="inlineStr"/>
+      <c r="O14" s="1" t="inlineStr"/>
+      <c r="P14" s="1" t="inlineStr"/>
+      <c r="Q14" s="1" t="inlineStr"/>
+      <c r="R14" s="1" t="inlineStr"/>
+      <c r="S14" s="1" t="inlineStr"/>
+      <c r="T14" s="1" t="inlineStr"/>
+      <c r="U14" s="1" t="inlineStr"/>
+      <c r="V14" s="1" t="inlineStr"/>
+      <c r="W14" s="1" t="inlineStr"/>
+      <c r="X14" s="1" t="inlineStr"/>
     </row>
     <row r="15" customHeight="1" ht="30">
       <c r="A15" s="1" t="inlineStr"/>
@@ -733,37 +1070,59 @@
         </is>
       </c>
       <c r="C15" s="11" t="inlineStr"/>
-      <c r="D15" s="11" t="inlineStr">
+      <c r="D15" s="11" t="inlineStr"/>
+      <c r="E15" s="11" t="inlineStr">
         <is>
           <r>
             <t xml:space="preserve">50</t>
           </r>
         </is>
       </c>
-      <c r="E15" s="1" t="inlineStr"/>
-      <c r="F15" s="1" t="inlineStr"/>
-      <c r="G15" s="1" t="inlineStr"/>
+      <c r="F15" s="11" t="inlineStr"/>
+      <c r="G15" s="11" t="inlineStr"/>
       <c r="H15" s="1" t="inlineStr"/>
       <c r="I15" s="1" t="inlineStr"/>
       <c r="J15" s="1" t="inlineStr"/>
       <c r="K15" s="1" t="inlineStr"/>
       <c r="L15" s="1" t="inlineStr"/>
       <c r="M15" s="1" t="inlineStr"/>
+      <c r="N15" s="1" t="inlineStr"/>
+      <c r="O15" s="1" t="inlineStr"/>
+      <c r="P15" s="1" t="inlineStr"/>
+      <c r="Q15" s="1" t="inlineStr"/>
+      <c r="R15" s="1" t="inlineStr"/>
+      <c r="S15" s="1" t="inlineStr"/>
+      <c r="T15" s="1" t="inlineStr"/>
+      <c r="U15" s="1" t="inlineStr"/>
+      <c r="V15" s="1" t="inlineStr"/>
+      <c r="W15" s="1" t="inlineStr"/>
+      <c r="X15" s="1" t="inlineStr"/>
     </row>
     <row r="16" customHeight="1" ht="30">
       <c r="A16" s="1" t="inlineStr"/>
       <c r="B16" s="12" t="inlineStr"/>
       <c r="C16" s="13" t="inlineStr"/>
       <c r="D16" s="14" t="inlineStr"/>
-      <c r="E16" s="1" t="inlineStr"/>
-      <c r="F16" s="1" t="inlineStr"/>
-      <c r="G16" s="1" t="inlineStr"/>
+      <c r="E16" s="12" t="inlineStr"/>
+      <c r="F16" s="13" t="inlineStr"/>
+      <c r="G16" s="14" t="inlineStr"/>
       <c r="H16" s="1" t="inlineStr"/>
       <c r="I16" s="1" t="inlineStr"/>
       <c r="J16" s="1" t="inlineStr"/>
       <c r="K16" s="1" t="inlineStr"/>
       <c r="L16" s="1" t="inlineStr"/>
       <c r="M16" s="1" t="inlineStr"/>
+      <c r="N16" s="1" t="inlineStr"/>
+      <c r="O16" s="1" t="inlineStr"/>
+      <c r="P16" s="1" t="inlineStr"/>
+      <c r="Q16" s="1" t="inlineStr"/>
+      <c r="R16" s="1" t="inlineStr"/>
+      <c r="S16" s="1" t="inlineStr"/>
+      <c r="T16" s="1" t="inlineStr"/>
+      <c r="U16" s="1" t="inlineStr"/>
+      <c r="V16" s="1" t="inlineStr"/>
+      <c r="W16" s="1" t="inlineStr"/>
+      <c r="X16" s="1" t="inlineStr"/>
     </row>
     <row r="17" customHeight="1" ht="30">
       <c r="A17" s="1" t="inlineStr"/>
@@ -775,22 +1134,33 @@
         </is>
       </c>
       <c r="C17" s="15" t="inlineStr"/>
-      <c r="D17" s="15" t="inlineStr">
+      <c r="D17" s="15" t="inlineStr"/>
+      <c r="E17" s="15" t="inlineStr">
         <is>
           <r>
             <t xml:space="preserve">300</t>
           </r>
         </is>
       </c>
-      <c r="E17" s="1" t="inlineStr"/>
-      <c r="F17" s="1" t="inlineStr"/>
-      <c r="G17" s="1" t="inlineStr"/>
+      <c r="F17" s="15" t="inlineStr"/>
+      <c r="G17" s="15" t="inlineStr"/>
       <c r="H17" s="1" t="inlineStr"/>
       <c r="I17" s="1" t="inlineStr"/>
       <c r="J17" s="1" t="inlineStr"/>
       <c r="K17" s="1" t="inlineStr"/>
       <c r="L17" s="1" t="inlineStr"/>
       <c r="M17" s="1" t="inlineStr"/>
+      <c r="N17" s="1" t="inlineStr"/>
+      <c r="O17" s="1" t="inlineStr"/>
+      <c r="P17" s="1" t="inlineStr"/>
+      <c r="Q17" s="1" t="inlineStr"/>
+      <c r="R17" s="1" t="inlineStr"/>
+      <c r="S17" s="1" t="inlineStr"/>
+      <c r="T17" s="1" t="inlineStr"/>
+      <c r="U17" s="1" t="inlineStr"/>
+      <c r="V17" s="1" t="inlineStr"/>
+      <c r="W17" s="1" t="inlineStr"/>
+      <c r="X17" s="1" t="inlineStr"/>
     </row>
     <row r="18" customHeight="1" ht="379">
       <c r="A18" s="1" t="inlineStr"/>
@@ -806,6 +1176,17 @@
       <c r="K18" s="1" t="inlineStr"/>
       <c r="L18" s="1" t="inlineStr"/>
       <c r="M18" s="1" t="inlineStr"/>
+      <c r="N18" s="1" t="inlineStr"/>
+      <c r="O18" s="1" t="inlineStr"/>
+      <c r="P18" s="1" t="inlineStr"/>
+      <c r="Q18" s="1" t="inlineStr"/>
+      <c r="R18" s="1" t="inlineStr"/>
+      <c r="S18" s="1" t="inlineStr"/>
+      <c r="T18" s="1" t="inlineStr"/>
+      <c r="U18" s="1" t="inlineStr"/>
+      <c r="V18" s="1" t="inlineStr"/>
+      <c r="W18" s="1" t="inlineStr"/>
+      <c r="X18" s="1" t="inlineStr"/>
     </row>
     <row r="19" customHeight="1" ht="30">
       <c r="A19" s="1" t="inlineStr"/>
@@ -815,24 +1196,35 @@
       <c r="E19" s="1" t="inlineStr"/>
       <c r="F19" s="1" t="inlineStr"/>
       <c r="G19" s="1" t="inlineStr"/>
-      <c r="H19" s="16" t="inlineStr">
+      <c r="H19" s="1" t="inlineStr"/>
+      <c r="I19" s="1" t="inlineStr"/>
+      <c r="J19" s="1" t="inlineStr"/>
+      <c r="K19" s="1" t="inlineStr"/>
+      <c r="L19" s="1" t="inlineStr"/>
+      <c r="M19" s="1" t="inlineStr"/>
+      <c r="N19" s="16" t="inlineStr">
         <is>
           <r>
             <t xml:space="preserve">Page 1</t>
           </r>
         </is>
       </c>
-      <c r="I19" s="16" t="inlineStr"/>
-      <c r="J19" s="17" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve"> of 2</t>
-          </r>
-        </is>
-      </c>
-      <c r="K19" s="17" t="inlineStr"/>
-      <c r="L19" s="17" t="inlineStr"/>
-      <c r="M19" s="1" t="inlineStr"/>
+      <c r="O19" s="16" t="inlineStr"/>
+      <c r="P19" s="17" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve"> of 3</t>
+          </r>
+        </is>
+      </c>
+      <c r="Q19" s="17" t="inlineStr"/>
+      <c r="R19" s="17" t="inlineStr"/>
+      <c r="S19" s="17" t="inlineStr"/>
+      <c r="T19" s="17" t="inlineStr"/>
+      <c r="U19" s="17" t="inlineStr"/>
+      <c r="V19" s="1" t="inlineStr"/>
+      <c r="W19" s="1" t="inlineStr"/>
+      <c r="X19" s="1" t="inlineStr"/>
     </row>
     <row r="20" customHeight="1" ht="20">
       <c r="A20" s="1" t="inlineStr"/>
@@ -848,6 +1240,17 @@
       <c r="K20" s="1" t="inlineStr"/>
       <c r="L20" s="1" t="inlineStr"/>
       <c r="M20" s="1" t="inlineStr"/>
+      <c r="N20" s="1" t="inlineStr"/>
+      <c r="O20" s="1" t="inlineStr"/>
+      <c r="P20" s="1" t="inlineStr"/>
+      <c r="Q20" s="1" t="inlineStr"/>
+      <c r="R20" s="1" t="inlineStr"/>
+      <c r="S20" s="1" t="inlineStr"/>
+      <c r="T20" s="1" t="inlineStr"/>
+      <c r="U20" s="1" t="inlineStr"/>
+      <c r="V20" s="1" t="inlineStr"/>
+      <c r="W20" s="1" t="inlineStr"/>
+      <c r="X20" s="1" t="inlineStr"/>
     </row>
     <row r="21" customHeight="1" ht="38">
       <c r="A21" s="1" t="inlineStr"/>
@@ -863,6 +1266,17 @@
       <c r="K21" s="1" t="inlineStr"/>
       <c r="L21" s="1" t="inlineStr"/>
       <c r="M21" s="1" t="inlineStr"/>
+      <c r="N21" s="1" t="inlineStr"/>
+      <c r="O21" s="1" t="inlineStr"/>
+      <c r="P21" s="1" t="inlineStr"/>
+      <c r="Q21" s="1" t="inlineStr"/>
+      <c r="R21" s="1" t="inlineStr"/>
+      <c r="S21" s="1" t="inlineStr"/>
+      <c r="T21" s="1" t="inlineStr"/>
+      <c r="U21" s="1" t="inlineStr"/>
+      <c r="V21" s="1" t="inlineStr"/>
+      <c r="W21" s="1" t="inlineStr"/>
+      <c r="X21" s="1" t="inlineStr"/>
     </row>
     <row r="22" customHeight="1" ht="1">
       <c r="A22" s="1" t="inlineStr"/>
@@ -877,9 +1291,20 @@
       <c r="J22" s="6" t="inlineStr"/>
       <c r="K22" s="6" t="inlineStr"/>
       <c r="L22" s="6" t="inlineStr"/>
-      <c r="M22" s="1" t="inlineStr"/>
-    </row>
-    <row r="23" customHeight="1" ht="368">
+      <c r="M22" s="6" t="inlineStr"/>
+      <c r="N22" s="6" t="inlineStr"/>
+      <c r="O22" s="6" t="inlineStr"/>
+      <c r="P22" s="6" t="inlineStr"/>
+      <c r="Q22" s="6" t="inlineStr"/>
+      <c r="R22" s="6" t="inlineStr"/>
+      <c r="S22" s="6" t="inlineStr"/>
+      <c r="T22" s="6" t="inlineStr"/>
+      <c r="U22" s="6" t="inlineStr"/>
+      <c r="V22" s="1" t="inlineStr"/>
+      <c r="W22" s="1" t="inlineStr"/>
+      <c r="X22" s="1" t="inlineStr"/>
+    </row>
+    <row r="23" customHeight="1" ht="753">
       <c r="A23" s="1" t="inlineStr"/>
       <c r="B23" s="1" t="inlineStr"/>
       <c r="C23" s="1" t="inlineStr"/>
@@ -893,23 +1318,57 @@
       <c r="K23" s="1" t="inlineStr"/>
       <c r="L23" s="1" t="inlineStr"/>
       <c r="M23" s="1" t="inlineStr"/>
-    </row>
-    <row r="24" customHeight="1" ht="200">
+      <c r="N23" s="1" t="inlineStr"/>
+      <c r="O23" s="1" t="inlineStr"/>
+      <c r="P23" s="1" t="inlineStr"/>
+      <c r="Q23" s="1" t="inlineStr"/>
+      <c r="R23" s="1" t="inlineStr"/>
+      <c r="S23" s="1" t="inlineStr"/>
+      <c r="T23" s="1" t="inlineStr"/>
+      <c r="U23" s="1" t="inlineStr"/>
+      <c r="V23" s="1" t="inlineStr"/>
+      <c r="W23" s="1" t="inlineStr"/>
+      <c r="X23" s="1" t="inlineStr"/>
+    </row>
+    <row r="24" customHeight="1" ht="30">
       <c r="A24" s="1" t="inlineStr"/>
-      <c r="B24" s="18" t="inlineStr"/>
-      <c r="C24" s="18" t="inlineStr"/>
-      <c r="D24" s="18" t="inlineStr"/>
+      <c r="B24" s="1" t="inlineStr"/>
+      <c r="C24" s="1" t="inlineStr"/>
+      <c r="D24" s="1" t="inlineStr"/>
       <c r="E24" s="1" t="inlineStr"/>
-      <c r="F24" s="18" t="inlineStr"/>
-      <c r="G24" s="18" t="inlineStr"/>
-      <c r="H24" s="18" t="inlineStr"/>
-      <c r="I24" s="18" t="inlineStr"/>
-      <c r="J24" s="18" t="inlineStr"/>
-      <c r="K24" s="18" t="inlineStr"/>
+      <c r="F24" s="1" t="inlineStr"/>
+      <c r="G24" s="1" t="inlineStr"/>
+      <c r="H24" s="1" t="inlineStr"/>
+      <c r="I24" s="1" t="inlineStr"/>
+      <c r="J24" s="1" t="inlineStr"/>
+      <c r="K24" s="1" t="inlineStr"/>
       <c r="L24" s="1" t="inlineStr"/>
       <c r="M24" s="1" t="inlineStr"/>
-    </row>
-    <row r="25" customHeight="1" ht="185">
+      <c r="N24" s="16" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Page 2</t>
+          </r>
+        </is>
+      </c>
+      <c r="O24" s="16" t="inlineStr"/>
+      <c r="P24" s="17" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve"> of 3</t>
+          </r>
+        </is>
+      </c>
+      <c r="Q24" s="17" t="inlineStr"/>
+      <c r="R24" s="17" t="inlineStr"/>
+      <c r="S24" s="17" t="inlineStr"/>
+      <c r="T24" s="17" t="inlineStr"/>
+      <c r="U24" s="17" t="inlineStr"/>
+      <c r="V24" s="1" t="inlineStr"/>
+      <c r="W24" s="1" t="inlineStr"/>
+      <c r="X24" s="1" t="inlineStr"/>
+    </row>
+    <row r="25" customHeight="1" ht="20">
       <c r="A25" s="1" t="inlineStr"/>
       <c r="B25" s="1" t="inlineStr"/>
       <c r="C25" s="1" t="inlineStr"/>
@@ -923,8 +1382,19 @@
       <c r="K25" s="1" t="inlineStr"/>
       <c r="L25" s="1" t="inlineStr"/>
       <c r="M25" s="1" t="inlineStr"/>
-    </row>
-    <row r="26" customHeight="1" ht="30">
+      <c r="N25" s="1" t="inlineStr"/>
+      <c r="O25" s="1" t="inlineStr"/>
+      <c r="P25" s="1" t="inlineStr"/>
+      <c r="Q25" s="1" t="inlineStr"/>
+      <c r="R25" s="1" t="inlineStr"/>
+      <c r="S25" s="1" t="inlineStr"/>
+      <c r="T25" s="1" t="inlineStr"/>
+      <c r="U25" s="1" t="inlineStr"/>
+      <c r="V25" s="1" t="inlineStr"/>
+      <c r="W25" s="1" t="inlineStr"/>
+      <c r="X25" s="1" t="inlineStr"/>
+    </row>
+    <row r="26" customHeight="1" ht="31">
       <c r="A26" s="1" t="inlineStr"/>
       <c r="B26" s="1" t="inlineStr"/>
       <c r="C26" s="1" t="inlineStr"/>
@@ -932,59 +1402,627 @@
       <c r="E26" s="1" t="inlineStr"/>
       <c r="F26" s="1" t="inlineStr"/>
       <c r="G26" s="1" t="inlineStr"/>
-      <c r="H26" s="16" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">Page 2</t>
-          </r>
-        </is>
-      </c>
-      <c r="I26" s="16" t="inlineStr"/>
-      <c r="J26" s="17" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve"> of 2</t>
-          </r>
-        </is>
-      </c>
-      <c r="K26" s="17" t="inlineStr"/>
-      <c r="L26" s="17" t="inlineStr"/>
+      <c r="H26" s="1" t="inlineStr"/>
+      <c r="I26" s="1" t="inlineStr"/>
+      <c r="J26" s="1" t="inlineStr"/>
+      <c r="K26" s="1" t="inlineStr"/>
+      <c r="L26" s="1" t="inlineStr"/>
       <c r="M26" s="1" t="inlineStr"/>
-    </row>
-    <row r="27" customHeight="1" ht="20">
+      <c r="N26" s="1" t="inlineStr"/>
+      <c r="O26" s="1" t="inlineStr"/>
+      <c r="P26" s="1" t="inlineStr"/>
+      <c r="Q26" s="1" t="inlineStr"/>
+      <c r="R26" s="1" t="inlineStr"/>
+      <c r="S26" s="1" t="inlineStr"/>
+      <c r="T26" s="1" t="inlineStr"/>
+      <c r="U26" s="1" t="inlineStr"/>
+      <c r="V26" s="1" t="inlineStr"/>
+      <c r="W26" s="1" t="inlineStr"/>
+      <c r="X26" s="1" t="inlineStr"/>
+    </row>
+    <row r="27" customHeight="1" ht="200">
       <c r="A27" s="1" t="inlineStr"/>
-      <c r="B27" s="1" t="inlineStr"/>
-      <c r="C27" s="1" t="inlineStr"/>
-      <c r="D27" s="1" t="inlineStr"/>
-      <c r="E27" s="1" t="inlineStr"/>
-      <c r="F27" s="1" t="inlineStr"/>
-      <c r="G27" s="1" t="inlineStr"/>
+      <c r="B27" s="18" t="inlineStr"/>
+      <c r="C27" s="18" t="inlineStr"/>
+      <c r="D27" s="18" t="inlineStr"/>
+      <c r="E27" s="18" t="inlineStr"/>
+      <c r="F27" s="18" t="inlineStr"/>
+      <c r="G27" s="18" t="inlineStr"/>
       <c r="H27" s="1" t="inlineStr"/>
-      <c r="I27" s="1" t="inlineStr"/>
-      <c r="J27" s="1" t="inlineStr"/>
-      <c r="K27" s="1" t="inlineStr"/>
-      <c r="L27" s="1" t="inlineStr"/>
-      <c r="M27" s="1" t="inlineStr"/>
+      <c r="I27" s="18" t="inlineStr"/>
+      <c r="J27" s="18" t="inlineStr"/>
+      <c r="K27" s="18" t="inlineStr"/>
+      <c r="L27" s="18" t="inlineStr"/>
+      <c r="M27" s="18" t="inlineStr"/>
+      <c r="N27" s="18" t="inlineStr"/>
+      <c r="O27" s="18" t="inlineStr"/>
+      <c r="P27" s="18" t="inlineStr"/>
+      <c r="Q27" s="18" t="inlineStr"/>
+      <c r="R27" s="18" t="inlineStr"/>
+      <c r="S27" s="18" t="inlineStr"/>
+      <c r="T27" s="18" t="inlineStr"/>
+      <c r="U27" s="1" t="inlineStr"/>
+      <c r="V27" s="1" t="inlineStr"/>
+      <c r="W27" s="1" t="inlineStr"/>
+      <c r="X27" s="1" t="inlineStr"/>
+    </row>
+    <row r="28" customHeight="1" ht="29">
+      <c r="A28" s="1" t="inlineStr"/>
+      <c r="B28" s="1" t="inlineStr"/>
+      <c r="C28" s="1" t="inlineStr"/>
+      <c r="D28" s="1" t="inlineStr"/>
+      <c r="E28" s="1" t="inlineStr"/>
+      <c r="F28" s="1" t="inlineStr"/>
+      <c r="G28" s="1" t="inlineStr"/>
+      <c r="H28" s="1" t="inlineStr"/>
+      <c r="I28" s="1" t="inlineStr"/>
+      <c r="J28" s="1" t="inlineStr"/>
+      <c r="K28" s="1" t="inlineStr"/>
+      <c r="L28" s="1" t="inlineStr"/>
+      <c r="M28" s="1" t="inlineStr"/>
+      <c r="N28" s="1" t="inlineStr"/>
+      <c r="O28" s="1" t="inlineStr"/>
+      <c r="P28" s="1" t="inlineStr"/>
+      <c r="Q28" s="1" t="inlineStr"/>
+      <c r="R28" s="1" t="inlineStr"/>
+      <c r="S28" s="1" t="inlineStr"/>
+      <c r="T28" s="1" t="inlineStr"/>
+      <c r="U28" s="1" t="inlineStr"/>
+      <c r="V28" s="1" t="inlineStr"/>
+      <c r="W28" s="1" t="inlineStr"/>
+      <c r="X28" s="1" t="inlineStr"/>
+    </row>
+    <row r="29" customHeight="1" ht="20">
+      <c r="A29" s="1" t="inlineStr"/>
+      <c r="B29" s="19" t="inlineStr"/>
+      <c r="C29" s="19" t="inlineStr"/>
+      <c r="D29" s="19" t="inlineStr"/>
+      <c r="E29" s="19" t="inlineStr"/>
+      <c r="F29" s="19" t="inlineStr"/>
+      <c r="G29" s="19" t="inlineStr"/>
+      <c r="H29" s="19" t="inlineStr"/>
+      <c r="I29" s="19" t="inlineStr"/>
+      <c r="J29" s="19" t="inlineStr"/>
+      <c r="K29" s="19" t="inlineStr"/>
+      <c r="L29" s="19" t="inlineStr"/>
+      <c r="M29" s="19" t="inlineStr"/>
+      <c r="N29" s="19" t="inlineStr"/>
+      <c r="O29" s="19" t="inlineStr"/>
+      <c r="P29" s="19" t="inlineStr"/>
+      <c r="Q29" s="19" t="inlineStr"/>
+      <c r="R29" s="19" t="inlineStr"/>
+      <c r="S29" s="19" t="inlineStr"/>
+      <c r="T29" s="19" t="inlineStr"/>
+      <c r="U29" s="19" t="inlineStr"/>
+      <c r="V29" s="19" t="inlineStr"/>
+      <c r="W29" s="19" t="inlineStr"/>
+      <c r="X29" s="19" t="inlineStr"/>
+    </row>
+    <row r="30" customHeight="1" ht="21">
+      <c r="A30" s="1" t="inlineStr"/>
+      <c r="B30" s="19" t="inlineStr"/>
+      <c r="C30" s="20" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">First Report</t>
+          </r>
+        </is>
+      </c>
+      <c r="D30" s="20" t="inlineStr"/>
+      <c r="E30" s="20" t="inlineStr"/>
+      <c r="F30" s="20" t="inlineStr"/>
+      <c r="G30" s="20" t="inlineStr"/>
+      <c r="H30" s="20" t="inlineStr"/>
+      <c r="I30" s="20" t="inlineStr"/>
+      <c r="J30" s="20" t="inlineStr"/>
+      <c r="K30" s="21" t="inlineStr"/>
+      <c r="L30" s="21" t="inlineStr"/>
+      <c r="M30" s="21" t="inlineStr"/>
+      <c r="N30" s="21" t="inlineStr"/>
+      <c r="O30" s="21" t="inlineStr"/>
+      <c r="P30" s="21" t="inlineStr"/>
+      <c r="Q30" s="21" t="inlineStr"/>
+      <c r="R30" s="21" t="inlineStr"/>
+      <c r="S30" s="21" t="inlineStr"/>
+      <c r="T30" s="21" t="inlineStr"/>
+      <c r="U30" s="21" t="inlineStr"/>
+      <c r="V30" s="21" t="inlineStr"/>
+      <c r="W30" s="21" t="inlineStr"/>
+      <c r="X30" s="19" t="inlineStr"/>
+    </row>
+    <row r="31" customHeight="1" ht="22">
+      <c r="A31" s="1" t="inlineStr"/>
+      <c r="B31" s="19" t="inlineStr"/>
+      <c r="C31" s="20" t="inlineStr"/>
+      <c r="D31" s="20" t="inlineStr"/>
+      <c r="E31" s="20" t="inlineStr"/>
+      <c r="F31" s="20" t="inlineStr"/>
+      <c r="G31" s="20" t="inlineStr"/>
+      <c r="H31" s="20" t="inlineStr"/>
+      <c r="I31" s="20" t="inlineStr"/>
+      <c r="J31" s="20" t="inlineStr"/>
+      <c r="K31" s="21" t="inlineStr"/>
+      <c r="L31" s="21" t="inlineStr"/>
+      <c r="M31" s="21" t="inlineStr"/>
+      <c r="N31" s="21" t="inlineStr"/>
+      <c r="O31" s="21" t="inlineStr"/>
+      <c r="P31" s="21" t="inlineStr"/>
+      <c r="Q31" s="21" t="inlineStr"/>
+      <c r="R31" s="22" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Raj</t>
+          </r>
+        </is>
+      </c>
+      <c r="S31" s="22" t="inlineStr"/>
+      <c r="T31" s="22" t="inlineStr"/>
+      <c r="U31" s="22" t="inlineStr"/>
+      <c r="V31" s="22" t="inlineStr"/>
+      <c r="W31" s="21" t="inlineStr"/>
+      <c r="X31" s="19" t="inlineStr"/>
+    </row>
+    <row r="32" customHeight="1" ht="8">
+      <c r="A32" s="1" t="inlineStr"/>
+      <c r="B32" s="19" t="inlineStr"/>
+      <c r="C32" s="21" t="inlineStr"/>
+      <c r="D32" s="21" t="inlineStr"/>
+      <c r="E32" s="21" t="inlineStr"/>
+      <c r="F32" s="21" t="inlineStr"/>
+      <c r="G32" s="21" t="inlineStr"/>
+      <c r="H32" s="21" t="inlineStr"/>
+      <c r="I32" s="21" t="inlineStr"/>
+      <c r="J32" s="21" t="inlineStr"/>
+      <c r="K32" s="21" t="inlineStr"/>
+      <c r="L32" s="21" t="inlineStr"/>
+      <c r="M32" s="21" t="inlineStr"/>
+      <c r="N32" s="21" t="inlineStr"/>
+      <c r="O32" s="21" t="inlineStr"/>
+      <c r="P32" s="21" t="inlineStr"/>
+      <c r="Q32" s="21" t="inlineStr"/>
+      <c r="R32" s="22" t="inlineStr"/>
+      <c r="S32" s="22" t="inlineStr"/>
+      <c r="T32" s="22" t="inlineStr"/>
+      <c r="U32" s="22" t="inlineStr"/>
+      <c r="V32" s="22" t="inlineStr"/>
+      <c r="W32" s="21" t="inlineStr"/>
+      <c r="X32" s="19" t="inlineStr"/>
+    </row>
+    <row r="33" customHeight="1" ht="21">
+      <c r="A33" s="1" t="inlineStr"/>
+      <c r="B33" s="19" t="inlineStr"/>
+      <c r="C33" s="19" t="inlineStr"/>
+      <c r="D33" s="19" t="inlineStr"/>
+      <c r="E33" s="19" t="inlineStr"/>
+      <c r="F33" s="19" t="inlineStr"/>
+      <c r="G33" s="19" t="inlineStr"/>
+      <c r="H33" s="19" t="inlineStr"/>
+      <c r="I33" s="19" t="inlineStr"/>
+      <c r="J33" s="19" t="inlineStr"/>
+      <c r="K33" s="19" t="inlineStr"/>
+      <c r="L33" s="19" t="inlineStr"/>
+      <c r="M33" s="19" t="inlineStr"/>
+      <c r="N33" s="19" t="inlineStr"/>
+      <c r="O33" s="19" t="inlineStr"/>
+      <c r="P33" s="19" t="inlineStr"/>
+      <c r="Q33" s="19" t="inlineStr"/>
+      <c r="R33" s="19" t="inlineStr"/>
+      <c r="S33" s="19" t="inlineStr"/>
+      <c r="T33" s="19" t="inlineStr"/>
+      <c r="U33" s="19" t="inlineStr"/>
+      <c r="V33" s="19" t="inlineStr"/>
+      <c r="W33" s="19" t="inlineStr"/>
+      <c r="X33" s="19" t="inlineStr"/>
+    </row>
+    <row r="34" customHeight="1" ht="13">
+      <c r="A34" s="1" t="inlineStr"/>
+      <c r="B34" s="1" t="inlineStr"/>
+      <c r="C34" s="1" t="inlineStr"/>
+      <c r="D34" s="1" t="inlineStr"/>
+      <c r="E34" s="1" t="inlineStr"/>
+      <c r="F34" s="1" t="inlineStr"/>
+      <c r="G34" s="1" t="inlineStr"/>
+      <c r="H34" s="1" t="inlineStr"/>
+      <c r="I34" s="1" t="inlineStr"/>
+      <c r="J34" s="1" t="inlineStr"/>
+      <c r="K34" s="1" t="inlineStr"/>
+      <c r="L34" s="1" t="inlineStr"/>
+      <c r="M34" s="1" t="inlineStr"/>
+      <c r="N34" s="1" t="inlineStr"/>
+      <c r="O34" s="1" t="inlineStr"/>
+      <c r="P34" s="1" t="inlineStr"/>
+      <c r="Q34" s="1" t="inlineStr"/>
+      <c r="R34" s="1" t="inlineStr"/>
+      <c r="S34" s="1" t="inlineStr"/>
+      <c r="T34" s="1" t="inlineStr"/>
+      <c r="U34" s="1" t="inlineStr"/>
+      <c r="V34" s="1" t="inlineStr"/>
+      <c r="W34" s="1" t="inlineStr"/>
+      <c r="X34" s="1" t="inlineStr"/>
+    </row>
+    <row r="35" customHeight="1" ht="20">
+      <c r="A35" s="1" t="inlineStr"/>
+      <c r="B35" s="1" t="inlineStr"/>
+      <c r="C35" s="23" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">ID</t>
+          </r>
+        </is>
+      </c>
+      <c r="D35" s="23" t="inlineStr"/>
+      <c r="E35" s="23" t="inlineStr"/>
+      <c r="F35" s="23" t="inlineStr"/>
+      <c r="G35" s="23" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">FIRSTNAME</t>
+          </r>
+        </is>
+      </c>
+      <c r="H35" s="23" t="inlineStr"/>
+      <c r="I35" s="23" t="inlineStr"/>
+      <c r="J35" s="23" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">LASTNAME</t>
+          </r>
+        </is>
+      </c>
+      <c r="K35" s="23" t="inlineStr"/>
+      <c r="L35" s="23" t="inlineStr"/>
+      <c r="M35" s="23" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">STREET</t>
+          </r>
+        </is>
+      </c>
+      <c r="N35" s="23" t="inlineStr"/>
+      <c r="O35" s="23" t="inlineStr"/>
+      <c r="P35" s="23" t="inlineStr"/>
+      <c r="Q35" s="23" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">CITY</t>
+          </r>
+        </is>
+      </c>
+      <c r="R35" s="23" t="inlineStr"/>
+      <c r="S35" s="23" t="inlineStr"/>
+      <c r="T35" s="23" t="inlineStr"/>
+      <c r="U35" s="23" t="inlineStr"/>
+      <c r="V35" s="23" t="inlineStr"/>
+      <c r="W35" s="23" t="inlineStr"/>
+      <c r="X35" s="1" t="inlineStr"/>
+    </row>
+    <row r="36" customHeight="1" ht="1">
+      <c r="A36" s="1" t="inlineStr"/>
+      <c r="B36" s="24" t="inlineStr"/>
+      <c r="C36" s="24" t="inlineStr"/>
+      <c r="D36" s="24" t="inlineStr"/>
+      <c r="E36" s="24" t="inlineStr"/>
+      <c r="F36" s="24" t="inlineStr"/>
+      <c r="G36" s="24" t="inlineStr"/>
+      <c r="H36" s="24" t="inlineStr"/>
+      <c r="I36" s="24" t="inlineStr"/>
+      <c r="J36" s="24" t="inlineStr"/>
+      <c r="K36" s="24" t="inlineStr"/>
+      <c r="L36" s="24" t="inlineStr"/>
+      <c r="M36" s="24" t="inlineStr"/>
+      <c r="N36" s="24" t="inlineStr"/>
+      <c r="O36" s="24" t="inlineStr"/>
+      <c r="P36" s="24" t="inlineStr"/>
+      <c r="Q36" s="24" t="inlineStr"/>
+      <c r="R36" s="24" t="inlineStr"/>
+      <c r="S36" s="24" t="inlineStr"/>
+      <c r="T36" s="24" t="inlineStr"/>
+      <c r="U36" s="24" t="inlineStr"/>
+      <c r="V36" s="24" t="inlineStr"/>
+      <c r="W36" s="24" t="inlineStr"/>
+      <c r="X36" s="24" t="inlineStr"/>
+    </row>
+    <row r="37" customHeight="1" ht="19">
+      <c r="A37" s="1" t="inlineStr"/>
+      <c r="B37" s="1" t="inlineStr"/>
+      <c r="C37" s="25" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">1</t>
+          </r>
+        </is>
+      </c>
+      <c r="D37" s="25" t="inlineStr"/>
+      <c r="E37" s="25" t="inlineStr"/>
+      <c r="F37" s="25" t="inlineStr"/>
+      <c r="G37" s="25" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Raj</t>
+          </r>
+        </is>
+      </c>
+      <c r="H37" s="25" t="inlineStr"/>
+      <c r="I37" s="25" t="inlineStr"/>
+      <c r="J37" s="25" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Joshi</t>
+          </r>
+        </is>
+      </c>
+      <c r="K37" s="25" t="inlineStr"/>
+      <c r="L37" s="25" t="inlineStr"/>
+      <c r="M37" s="25" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Happy Street</t>
+          </r>
+        </is>
+      </c>
+      <c r="N37" s="25" t="inlineStr"/>
+      <c r="O37" s="25" t="inlineStr"/>
+      <c r="P37" s="25" t="inlineStr"/>
+      <c r="Q37" s="25" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Delhi</t>
+          </r>
+        </is>
+      </c>
+      <c r="R37" s="25" t="inlineStr"/>
+      <c r="S37" s="25" t="inlineStr"/>
+      <c r="T37" s="25" t="inlineStr"/>
+      <c r="U37" s="25" t="inlineStr"/>
+      <c r="V37" s="25" t="inlineStr"/>
+      <c r="W37" s="25" t="inlineStr"/>
+      <c r="X37" s="1" t="inlineStr"/>
+    </row>
+    <row r="38" customHeight="1" ht="1">
+      <c r="A38" s="1" t="inlineStr"/>
+      <c r="B38" s="1" t="inlineStr"/>
+      <c r="C38" s="25" t="inlineStr"/>
+      <c r="D38" s="25" t="inlineStr"/>
+      <c r="E38" s="25" t="inlineStr"/>
+      <c r="F38" s="25" t="inlineStr"/>
+      <c r="G38" s="25" t="inlineStr"/>
+      <c r="H38" s="25" t="inlineStr"/>
+      <c r="I38" s="25" t="inlineStr"/>
+      <c r="J38" s="25" t="inlineStr"/>
+      <c r="K38" s="25" t="inlineStr"/>
+      <c r="L38" s="25" t="inlineStr"/>
+      <c r="M38" s="25" t="inlineStr"/>
+      <c r="N38" s="25" t="inlineStr"/>
+      <c r="O38" s="25" t="inlineStr"/>
+      <c r="P38" s="25" t="inlineStr"/>
+      <c r="Q38" s="25" t="inlineStr"/>
+      <c r="R38" s="25" t="inlineStr"/>
+      <c r="S38" s="25" t="inlineStr"/>
+      <c r="T38" s="25" t="inlineStr"/>
+      <c r="U38" s="25" t="inlineStr"/>
+      <c r="V38" s="25" t="inlineStr"/>
+      <c r="W38" s="25" t="inlineStr"/>
+      <c r="X38" s="1" t="inlineStr"/>
+    </row>
+    <row r="39" customHeight="1" ht="19">
+      <c r="A39" s="1" t="inlineStr"/>
+      <c r="B39" s="1" t="inlineStr"/>
+      <c r="C39" s="25" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">2</t>
+          </r>
+        </is>
+      </c>
+      <c r="D39" s="25" t="inlineStr"/>
+      <c r="E39" s="25" t="inlineStr"/>
+      <c r="F39" s="25" t="inlineStr"/>
+      <c r="G39" s="25" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Peter</t>
+          </r>
+        </is>
+      </c>
+      <c r="H39" s="25" t="inlineStr"/>
+      <c r="I39" s="25" t="inlineStr"/>
+      <c r="J39" s="25" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Smith</t>
+          </r>
+        </is>
+      </c>
+      <c r="K39" s="25" t="inlineStr"/>
+      <c r="L39" s="25" t="inlineStr"/>
+      <c r="M39" s="25" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Any Street</t>
+          </r>
+        </is>
+      </c>
+      <c r="N39" s="25" t="inlineStr"/>
+      <c r="O39" s="25" t="inlineStr"/>
+      <c r="P39" s="25" t="inlineStr"/>
+      <c r="Q39" s="25" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Mumbai</t>
+          </r>
+        </is>
+      </c>
+      <c r="R39" s="25" t="inlineStr"/>
+      <c r="S39" s="25" t="inlineStr"/>
+      <c r="T39" s="25" t="inlineStr"/>
+      <c r="U39" s="25" t="inlineStr"/>
+      <c r="V39" s="25" t="inlineStr"/>
+      <c r="W39" s="25" t="inlineStr"/>
+      <c r="X39" s="1" t="inlineStr"/>
+    </row>
+    <row r="40" customHeight="1" ht="1">
+      <c r="A40" s="1" t="inlineStr"/>
+      <c r="B40" s="1" t="inlineStr"/>
+      <c r="C40" s="25" t="inlineStr"/>
+      <c r="D40" s="25" t="inlineStr"/>
+      <c r="E40" s="25" t="inlineStr"/>
+      <c r="F40" s="25" t="inlineStr"/>
+      <c r="G40" s="25" t="inlineStr"/>
+      <c r="H40" s="25" t="inlineStr"/>
+      <c r="I40" s="25" t="inlineStr"/>
+      <c r="J40" s="25" t="inlineStr"/>
+      <c r="K40" s="25" t="inlineStr"/>
+      <c r="L40" s="25" t="inlineStr"/>
+      <c r="M40" s="25" t="inlineStr"/>
+      <c r="N40" s="25" t="inlineStr"/>
+      <c r="O40" s="25" t="inlineStr"/>
+      <c r="P40" s="25" t="inlineStr"/>
+      <c r="Q40" s="25" t="inlineStr"/>
+      <c r="R40" s="25" t="inlineStr"/>
+      <c r="S40" s="25" t="inlineStr"/>
+      <c r="T40" s="25" t="inlineStr"/>
+      <c r="U40" s="25" t="inlineStr"/>
+      <c r="V40" s="25" t="inlineStr"/>
+      <c r="W40" s="25" t="inlineStr"/>
+      <c r="X40" s="1" t="inlineStr"/>
+    </row>
+    <row r="41" customHeight="1" ht="4">
+      <c r="A41" s="1" t="inlineStr"/>
+      <c r="B41" s="1" t="inlineStr"/>
+      <c r="C41" s="1" t="inlineStr"/>
+      <c r="D41" s="1" t="inlineStr"/>
+      <c r="E41" s="1" t="inlineStr"/>
+      <c r="F41" s="1" t="inlineStr"/>
+      <c r="G41" s="1" t="inlineStr"/>
+      <c r="H41" s="1" t="inlineStr"/>
+      <c r="I41" s="1" t="inlineStr"/>
+      <c r="J41" s="1" t="inlineStr"/>
+      <c r="K41" s="1" t="inlineStr"/>
+      <c r="L41" s="1" t="inlineStr"/>
+      <c r="M41" s="1" t="inlineStr"/>
+      <c r="N41" s="1" t="inlineStr"/>
+      <c r="O41" s="1" t="inlineStr"/>
+      <c r="P41" s="1" t="inlineStr"/>
+      <c r="Q41" s="1" t="inlineStr"/>
+      <c r="R41" s="1" t="inlineStr"/>
+      <c r="S41" s="1" t="inlineStr"/>
+      <c r="T41" s="1" t="inlineStr"/>
+      <c r="U41" s="1" t="inlineStr"/>
+      <c r="V41" s="1" t="inlineStr"/>
+      <c r="W41" s="1" t="inlineStr"/>
+      <c r="X41" s="1" t="inlineStr"/>
+    </row>
+    <row r="42" customHeight="1" ht="13">
+      <c r="A42" s="1" t="inlineStr"/>
+      <c r="B42" s="1" t="inlineStr"/>
+      <c r="C42" s="17" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">miércoles 22 junio </t>
+          </r>
+        </is>
+      </c>
+      <c r="D42" s="17" t="inlineStr"/>
+      <c r="E42" s="17" t="inlineStr"/>
+      <c r="F42" s="1" t="inlineStr"/>
+      <c r="G42" s="1" t="inlineStr"/>
+      <c r="H42" s="1" t="inlineStr"/>
+      <c r="I42" s="1" t="inlineStr"/>
+      <c r="J42" s="1" t="inlineStr"/>
+      <c r="K42" s="1" t="inlineStr"/>
+      <c r="L42" s="1" t="inlineStr"/>
+      <c r="M42" s="1" t="inlineStr"/>
+      <c r="N42" s="1" t="inlineStr"/>
+      <c r="O42" s="1" t="inlineStr"/>
+      <c r="P42" s="1" t="inlineStr"/>
+      <c r="Q42" s="1" t="inlineStr"/>
+      <c r="R42" s="1" t="inlineStr"/>
+      <c r="S42" s="1" t="inlineStr"/>
+      <c r="T42" s="26" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve"> 1</t>
+          </r>
+        </is>
+      </c>
+      <c r="U42" s="26" t="inlineStr"/>
+      <c r="V42" s="26" t="inlineStr"/>
+      <c r="W42" s="26" t="inlineStr"/>
+      <c r="X42" s="1" t="inlineStr"/>
+    </row>
+    <row r="43" customHeight="1" ht="399">
+      <c r="A43" s="1" t="inlineStr"/>
+      <c r="B43" s="1" t="inlineStr"/>
+      <c r="C43" s="1" t="inlineStr"/>
+      <c r="D43" s="1" t="inlineStr"/>
+      <c r="E43" s="1" t="inlineStr"/>
+      <c r="F43" s="1" t="inlineStr"/>
+      <c r="G43" s="1" t="inlineStr"/>
+      <c r="H43" s="1" t="inlineStr"/>
+      <c r="I43" s="1" t="inlineStr"/>
+      <c r="J43" s="1" t="inlineStr"/>
+      <c r="K43" s="1" t="inlineStr"/>
+      <c r="L43" s="1" t="inlineStr"/>
+      <c r="M43" s="1" t="inlineStr"/>
+      <c r="N43" s="1" t="inlineStr"/>
+      <c r="O43" s="1" t="inlineStr"/>
+      <c r="P43" s="1" t="inlineStr"/>
+      <c r="Q43" s="1" t="inlineStr"/>
+      <c r="R43" s="1" t="inlineStr"/>
+      <c r="S43" s="1" t="inlineStr"/>
+      <c r="T43" s="1" t="inlineStr"/>
+      <c r="U43" s="1" t="inlineStr"/>
+      <c r="V43" s="1" t="inlineStr"/>
+      <c r="W43" s="1" t="inlineStr"/>
+      <c r="X43" s="1" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="B7:L7"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="B22:L22"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="F24:K24"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="B2:C5"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="O5:R5"/>
+    <mergeCell ref="B7:U7"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="P19:U19"/>
+    <mergeCell ref="B22:U22"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="P24:U24"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="I27:T27"/>
+    <mergeCell ref="C30:J31"/>
+    <mergeCell ref="R31:V32"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="J35:L35"/>
+    <mergeCell ref="M35:P35"/>
+    <mergeCell ref="Q35:W35"/>
+    <mergeCell ref="B36:X36"/>
+    <mergeCell ref="C37:F38"/>
+    <mergeCell ref="G37:I38"/>
+    <mergeCell ref="J37:L38"/>
+    <mergeCell ref="M37:P38"/>
+    <mergeCell ref="Q37:W38"/>
+    <mergeCell ref="C39:F40"/>
+    <mergeCell ref="G39:I40"/>
+    <mergeCell ref="J39:L40"/>
+    <mergeCell ref="M39:P40"/>
+    <mergeCell ref="Q39:W40"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="T42:W42"/>
   </mergeCells>
   <pageMargins left="0.0" right="0.0" top="0.0" bottom="0.00" header="0.0" footer="0.0"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>